<commit_message>
adding poc for using material layout with the material framework
</commit_message>
<xml_diff>
--- a/Layout/metric-and-keylines.xlsx
+++ b/Layout/metric-and-keylines.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -62,6 +62,51 @@
   </si>
   <si>
     <t>Toolbar height</t>
+  </si>
+  <si>
+    <t>Dividers</t>
+  </si>
+  <si>
+    <t>Primary Text</t>
+  </si>
+  <si>
+    <t>Secondary Text</t>
+  </si>
+  <si>
+    <t>Disabled/hint Text</t>
+  </si>
+  <si>
+    <t>White Opacity</t>
+  </si>
+  <si>
+    <t>Dark Opacity</t>
+  </si>
+  <si>
+    <t>Active Icon</t>
+  </si>
+  <si>
+    <t>Inactive Icon</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Desktop</t>
+  </si>
+  <si>
+    <t>App Bar</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Subtitle</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Caption</t>
   </si>
 </sst>
 </file>
@@ -412,17 +457,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,8 +487,27 @@
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -449,8 +520,26 @@
       <c r="D2">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2">
+        <v>87</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -463,8 +552,26 @@
       <c r="D3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>54</v>
+      </c>
+      <c r="H3">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3">
+        <v>14</v>
+      </c>
+      <c r="L3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -477,8 +584,26 @@
       <c r="D4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>38</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4">
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -491,8 +616,26 @@
       <c r="D5">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5">
+        <v>14</v>
+      </c>
+      <c r="L5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -505,8 +648,26 @@
       <c r="D6">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6">
+        <v>54</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
+      <c r="L6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -519,8 +680,17 @@
       <c r="D7">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -534,7 +704,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -548,7 +718,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -562,7 +732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -576,7 +746,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>

</xml_diff>